<commit_message>
readme correction & final file addition
</commit_message>
<xml_diff>
--- a/Data/Clean/dictionary_big_cities_census.xlsx
+++ b/Data/Clean/dictionary_big_cities_census.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reffet/Desktop/IESEG/techniques_de_recherche/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reffet/Desktop/IESEG/techniques_de_recherche/project_econometrics/Data/Clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DC9EC8-BC5D-3C4A-B027-7CB42ADA6484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04309DD1-09D5-6947-BAFF-E9FF2AFED35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15220" xr2:uid="{9252A554-32EC-D94B-B415-6CF0636FA536}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="325">
   <si>
     <t>352xx</t>
   </si>
@@ -1006,16 +1006,10 @@
     <t>820xx</t>
   </si>
   <si>
-    <t>Encoding</t>
+    <t>zip_code</t>
   </si>
   <si>
     <t>big_city</t>
-  </si>
-  <si>
-    <t>column</t>
-  </si>
-  <si>
-    <t>Zip</t>
   </si>
 </sst>
 </file>
@@ -1379,7 +1373,7 @@
   <dimension ref="A1:C324"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1389,14 +1383,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>325</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1405,9 +1397,7 @@
       <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1416,9 +1406,7 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1427,9 +1415,7 @@
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1438,9 +1424,7 @@
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1449,9 +1433,7 @@
       <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -1460,9 +1442,7 @@
       <c r="B7" s="2">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -1471,9 +1451,7 @@
       <c r="B8" s="2">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1482,9 +1460,7 @@
       <c r="B9" s="2">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -1493,9 +1469,7 @@
       <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -1504,9 +1478,7 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -1515,9 +1487,7 @@
       <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -1526,9 +1496,7 @@
       <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -1537,9 +1505,7 @@
       <c r="B14" s="2">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -1548,9 +1514,7 @@
       <c r="B15" s="2">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1559,9 +1523,7 @@
       <c r="B16" s="2">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -1570,9 +1532,7 @@
       <c r="B17" s="2">
         <v>1</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
@@ -1581,9 +1541,7 @@
       <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -1592,9 +1550,7 @@
       <c r="B19" s="2">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -1603,9 +1559,7 @@
       <c r="B20" s="2">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -1614,9 +1568,7 @@
       <c r="B21" s="2">
         <v>1</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -1625,9 +1577,7 @@
       <c r="B22" s="2">
         <v>1</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
@@ -1636,9 +1586,7 @@
       <c r="B23" s="2">
         <v>1</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -1647,9 +1595,7 @@
       <c r="B24" s="2">
         <v>1</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -1658,9 +1604,7 @@
       <c r="B25" s="2">
         <v>1</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -1669,9 +1613,7 @@
       <c r="B26" s="2">
         <v>1</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -1680,9 +1622,7 @@
       <c r="B27" s="2">
         <v>1</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
@@ -1691,9 +1631,7 @@
       <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -1702,9 +1640,7 @@
       <c r="B29" s="2">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -1713,9 +1649,7 @@
       <c r="B30" s="2">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
@@ -1724,9 +1658,7 @@
       <c r="B31" s="2">
         <v>1</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
@@ -1735,9 +1667,7 @@
       <c r="B32" s="2">
         <v>1</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
@@ -1746,9 +1676,7 @@
       <c r="B33" s="2">
         <v>1</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
@@ -1757,9 +1685,7 @@
       <c r="B34" s="2">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
@@ -1768,9 +1694,7 @@
       <c r="B35" s="2">
         <v>1</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
@@ -1779,9 +1703,7 @@
       <c r="B36" s="2">
         <v>1</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
@@ -1790,9 +1712,7 @@
       <c r="B37" s="2">
         <v>1</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
@@ -1801,9 +1721,7 @@
       <c r="B38" s="2">
         <v>1</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
@@ -1812,9 +1730,7 @@
       <c r="B39" s="2">
         <v>1</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
@@ -1823,9 +1739,7 @@
       <c r="B40" s="2">
         <v>1</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
@@ -1834,9 +1748,7 @@
       <c r="B41" s="2">
         <v>1</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
@@ -1845,9 +1757,7 @@
       <c r="B42" s="2">
         <v>1</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
@@ -1856,9 +1766,7 @@
       <c r="B43" s="2">
         <v>1</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
@@ -1867,9 +1775,7 @@
       <c r="B44" s="2">
         <v>1</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
@@ -1878,9 +1784,7 @@
       <c r="B45" s="2">
         <v>1</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
@@ -1889,9 +1793,7 @@
       <c r="B46" s="2">
         <v>1</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
@@ -1900,9 +1802,7 @@
       <c r="B47" s="2">
         <v>1</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
@@ -1911,9 +1811,7 @@
       <c r="B48" s="2">
         <v>1</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -1922,9 +1820,7 @@
       <c r="B49" s="2">
         <v>1</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
@@ -1933,9 +1829,7 @@
       <c r="B50" s="2">
         <v>1</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
@@ -1944,9 +1838,7 @@
       <c r="B51" s="2">
         <v>1</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
@@ -1955,9 +1847,7 @@
       <c r="B52" s="2">
         <v>1</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
@@ -1966,9 +1856,7 @@
       <c r="B53" s="2">
         <v>1</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
@@ -1977,9 +1865,7 @@
       <c r="B54" s="2">
         <v>1</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
@@ -1988,9 +1874,7 @@
       <c r="B55" s="2">
         <v>1</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
@@ -1999,9 +1883,7 @@
       <c r="B56" s="2">
         <v>1</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
@@ -2010,9 +1892,7 @@
       <c r="B57" s="2">
         <v>1</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
@@ -2021,9 +1901,7 @@
       <c r="B58" s="2">
         <v>1</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
@@ -2032,9 +1910,7 @@
       <c r="B59" s="2">
         <v>1</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -2043,9 +1919,7 @@
       <c r="B60" s="2">
         <v>1</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
@@ -2054,9 +1928,7 @@
       <c r="B61" s="2">
         <v>1</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
@@ -2065,9 +1937,7 @@
       <c r="B62" s="2">
         <v>1</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
@@ -2076,9 +1946,7 @@
       <c r="B63" s="2">
         <v>1</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
@@ -2087,9 +1955,7 @@
       <c r="B64" s="2">
         <v>1</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C64" s="1"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
@@ -2098,9 +1964,7 @@
       <c r="B65" s="2">
         <v>1</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
@@ -2109,9 +1973,7 @@
       <c r="B66" s="2">
         <v>1</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C66" s="1"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
@@ -2120,9 +1982,7 @@
       <c r="B67" s="2">
         <v>1</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
@@ -2131,9 +1991,7 @@
       <c r="B68" s="2">
         <v>1</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C68" s="1"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
@@ -2142,9 +2000,7 @@
       <c r="B69" s="2">
         <v>1</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
@@ -2153,9 +2009,7 @@
       <c r="B70" s="2">
         <v>1</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
@@ -2164,9 +2018,7 @@
       <c r="B71" s="2">
         <v>1</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
@@ -2175,9 +2027,7 @@
       <c r="B72" s="2">
         <v>1</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
@@ -2186,9 +2036,7 @@
       <c r="B73" s="2">
         <v>1</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
@@ -2197,9 +2045,7 @@
       <c r="B74" s="2">
         <v>1</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
@@ -2208,9 +2054,7 @@
       <c r="B75" s="2">
         <v>1</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
@@ -2219,9 +2063,7 @@
       <c r="B76" s="2">
         <v>1</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
@@ -2230,9 +2072,7 @@
       <c r="B77" s="2">
         <v>1</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
@@ -2241,9 +2081,7 @@
       <c r="B78" s="2">
         <v>1</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C78" s="1"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
@@ -2252,9 +2090,7 @@
       <c r="B79" s="2">
         <v>1</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
@@ -2263,9 +2099,7 @@
       <c r="B80" s="2">
         <v>1</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C80" s="1"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
@@ -2274,9 +2108,7 @@
       <c r="B81" s="2">
         <v>1</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
@@ -2285,9 +2117,7 @@
       <c r="B82" s="2">
         <v>1</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C82" s="1"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
@@ -2296,9 +2126,7 @@
       <c r="B83" s="2">
         <v>1</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
@@ -2307,9 +2135,7 @@
       <c r="B84" s="2">
         <v>1</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C84" s="1"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
@@ -2318,9 +2144,7 @@
       <c r="B85" s="2">
         <v>1</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C85" s="1"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
@@ -2329,9 +2153,7 @@
       <c r="B86" s="2">
         <v>1</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C86" s="1"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
@@ -2340,9 +2162,7 @@
       <c r="B87" s="2">
         <v>1</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C87" s="1"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
@@ -2351,9 +2171,7 @@
       <c r="B88" s="2">
         <v>1</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C88" s="1"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
@@ -2362,9 +2180,7 @@
       <c r="B89" s="2">
         <v>1</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C89" s="1"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
@@ -2373,9 +2189,7 @@
       <c r="B90" s="2">
         <v>1</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C90" s="1"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
@@ -2384,9 +2198,7 @@
       <c r="B91" s="2">
         <v>1</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C91" s="1"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
@@ -2395,9 +2207,7 @@
       <c r="B92" s="2">
         <v>1</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C92" s="1"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
@@ -2406,9 +2216,7 @@
       <c r="B93" s="2">
         <v>1</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C93" s="1"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
@@ -2417,9 +2225,7 @@
       <c r="B94" s="2">
         <v>1</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C94" s="1"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
@@ -2428,9 +2234,7 @@
       <c r="B95" s="2">
         <v>1</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C95" s="1"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
@@ -2439,9 +2243,7 @@
       <c r="B96" s="2">
         <v>1</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C96" s="1"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
@@ -2450,9 +2252,7 @@
       <c r="B97" s="2">
         <v>1</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C97" s="1"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
@@ -2461,9 +2261,7 @@
       <c r="B98" s="2">
         <v>1</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C98" s="1"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
@@ -2472,9 +2270,7 @@
       <c r="B99" s="2">
         <v>1</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
@@ -2483,9 +2279,7 @@
       <c r="B100" s="2">
         <v>1</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
@@ -2494,9 +2288,7 @@
       <c r="B101" s="2">
         <v>1</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C101" s="1"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
@@ -2505,9 +2297,7 @@
       <c r="B102" s="2">
         <v>1</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C102" s="1"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
@@ -2516,9 +2306,7 @@
       <c r="B103" s="2">
         <v>1</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C103" s="1"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
@@ -2527,9 +2315,7 @@
       <c r="B104" s="2">
         <v>1</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C104" s="1"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
@@ -2538,9 +2324,7 @@
       <c r="B105" s="2">
         <v>1</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C105" s="1"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
@@ -2549,9 +2333,7 @@
       <c r="B106" s="2">
         <v>1</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C106" s="1"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
@@ -2560,9 +2342,7 @@
       <c r="B107" s="2">
         <v>1</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
@@ -2571,9 +2351,7 @@
       <c r="B108" s="2">
         <v>1</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C108" s="1"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
@@ -2582,9 +2360,7 @@
       <c r="B109" s="2">
         <v>1</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C109" s="1"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
@@ -2593,9 +2369,7 @@
       <c r="B110" s="2">
         <v>1</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C110" s="1"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
@@ -2604,9 +2378,7 @@
       <c r="B111" s="2">
         <v>1</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C111" s="1"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
@@ -2615,9 +2387,7 @@
       <c r="B112" s="2">
         <v>1</v>
       </c>
-      <c r="C112" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C112" s="1"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
@@ -2626,9 +2396,7 @@
       <c r="B113" s="2">
         <v>1</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C113" s="1"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
@@ -2637,9 +2405,7 @@
       <c r="B114" s="2">
         <v>1</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C114" s="1"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
@@ -2648,9 +2414,7 @@
       <c r="B115" s="2">
         <v>1</v>
       </c>
-      <c r="C115" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C115" s="1"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
@@ -2659,9 +2423,7 @@
       <c r="B116" s="2">
         <v>1</v>
       </c>
-      <c r="C116" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C116" s="1"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
@@ -2670,9 +2432,7 @@
       <c r="B117" s="2">
         <v>1</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C117" s="1"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
@@ -2681,9 +2441,7 @@
       <c r="B118" s="2">
         <v>1</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C118" s="1"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
@@ -2692,9 +2450,7 @@
       <c r="B119" s="2">
         <v>1</v>
       </c>
-      <c r="C119" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C119" s="1"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
@@ -2703,9 +2459,7 @@
       <c r="B120" s="2">
         <v>1</v>
       </c>
-      <c r="C120" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C120" s="1"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
@@ -2714,9 +2468,7 @@
       <c r="B121" s="2">
         <v>1</v>
       </c>
-      <c r="C121" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C121" s="1"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
@@ -2725,9 +2477,7 @@
       <c r="B122" s="2">
         <v>1</v>
       </c>
-      <c r="C122" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C122" s="1"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
@@ -2736,9 +2486,7 @@
       <c r="B123" s="2">
         <v>1</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C123" s="1"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
@@ -2747,9 +2495,7 @@
       <c r="B124" s="2">
         <v>1</v>
       </c>
-      <c r="C124" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C124" s="1"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
@@ -2758,9 +2504,7 @@
       <c r="B125" s="2">
         <v>1</v>
       </c>
-      <c r="C125" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C125" s="1"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
@@ -2769,9 +2513,7 @@
       <c r="B126" s="2">
         <v>1</v>
       </c>
-      <c r="C126" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C126" s="1"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
@@ -2780,9 +2522,7 @@
       <c r="B127" s="2">
         <v>1</v>
       </c>
-      <c r="C127" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C127" s="1"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
@@ -2791,9 +2531,7 @@
       <c r="B128" s="2">
         <v>1</v>
       </c>
-      <c r="C128" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C128" s="1"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
@@ -2802,9 +2540,7 @@
       <c r="B129" s="2">
         <v>1</v>
       </c>
-      <c r="C129" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C129" s="1"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
@@ -2813,9 +2549,7 @@
       <c r="B130" s="2">
         <v>1</v>
       </c>
-      <c r="C130" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C130" s="1"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
@@ -2824,9 +2558,7 @@
       <c r="B131" s="2">
         <v>1</v>
       </c>
-      <c r="C131" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C131" s="1"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
@@ -2835,9 +2567,7 @@
       <c r="B132" s="2">
         <v>1</v>
       </c>
-      <c r="C132" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C132" s="1"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
@@ -2846,9 +2576,7 @@
       <c r="B133" s="2">
         <v>1</v>
       </c>
-      <c r="C133" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C133" s="1"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
@@ -2857,9 +2585,7 @@
       <c r="B134" s="2">
         <v>1</v>
       </c>
-      <c r="C134" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C134" s="1"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
@@ -2868,9 +2594,7 @@
       <c r="B135" s="2">
         <v>1</v>
       </c>
-      <c r="C135" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C135" s="1"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
@@ -2879,9 +2603,7 @@
       <c r="B136" s="2">
         <v>1</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C136" s="1"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
@@ -2890,9 +2612,7 @@
       <c r="B137" s="2">
         <v>1</v>
       </c>
-      <c r="C137" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C137" s="1"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
@@ -2901,9 +2621,7 @@
       <c r="B138" s="2">
         <v>1</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C138" s="1"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
@@ -2912,9 +2630,7 @@
       <c r="B139" s="2">
         <v>1</v>
       </c>
-      <c r="C139" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C139" s="1"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
@@ -2923,9 +2639,7 @@
       <c r="B140" s="2">
         <v>1</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C140" s="1"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
@@ -2934,9 +2648,7 @@
       <c r="B141" s="2">
         <v>1</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C141" s="1"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
@@ -2945,9 +2657,7 @@
       <c r="B142" s="2">
         <v>1</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C142" s="1"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
@@ -2956,9 +2666,7 @@
       <c r="B143" s="2">
         <v>1</v>
       </c>
-      <c r="C143" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C143" s="1"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
@@ -2967,9 +2675,7 @@
       <c r="B144" s="2">
         <v>1</v>
       </c>
-      <c r="C144" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C144" s="1"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
@@ -2978,9 +2684,7 @@
       <c r="B145" s="2">
         <v>1</v>
       </c>
-      <c r="C145" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C145" s="1"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
@@ -2989,9 +2693,7 @@
       <c r="B146" s="2">
         <v>1</v>
       </c>
-      <c r="C146" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C146" s="1"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
@@ -3000,9 +2702,7 @@
       <c r="B147" s="2">
         <v>1</v>
       </c>
-      <c r="C147" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C147" s="1"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
@@ -3011,9 +2711,7 @@
       <c r="B148" s="2">
         <v>1</v>
       </c>
-      <c r="C148" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C148" s="1"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
@@ -3022,9 +2720,7 @@
       <c r="B149" s="2">
         <v>1</v>
       </c>
-      <c r="C149" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C149" s="1"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
@@ -3033,9 +2729,7 @@
       <c r="B150" s="2">
         <v>1</v>
       </c>
-      <c r="C150" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C150" s="1"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
@@ -3044,9 +2738,7 @@
       <c r="B151" s="2">
         <v>1</v>
       </c>
-      <c r="C151" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C151" s="1"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
@@ -3055,9 +2747,7 @@
       <c r="B152" s="2">
         <v>1</v>
       </c>
-      <c r="C152" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C152" s="1"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
@@ -3066,9 +2756,7 @@
       <c r="B153" s="2">
         <v>1</v>
       </c>
-      <c r="C153" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C153" s="1"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
@@ -3077,9 +2765,7 @@
       <c r="B154" s="2">
         <v>1</v>
       </c>
-      <c r="C154" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C154" s="1"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
@@ -3088,9 +2774,7 @@
       <c r="B155" s="2">
         <v>1</v>
       </c>
-      <c r="C155" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C155" s="1"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
@@ -3099,9 +2783,7 @@
       <c r="B156" s="2">
         <v>1</v>
       </c>
-      <c r="C156" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C156" s="1"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
@@ -3110,9 +2792,7 @@
       <c r="B157" s="2">
         <v>1</v>
       </c>
-      <c r="C157" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C157" s="1"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
@@ -3121,9 +2801,7 @@
       <c r="B158" s="2">
         <v>1</v>
       </c>
-      <c r="C158" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C158" s="1"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
@@ -3132,9 +2810,7 @@
       <c r="B159" s="2">
         <v>1</v>
       </c>
-      <c r="C159" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C159" s="1"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
@@ -3143,9 +2819,7 @@
       <c r="B160" s="2">
         <v>1</v>
       </c>
-      <c r="C160" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C160" s="1"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
@@ -3154,9 +2828,7 @@
       <c r="B161" s="2">
         <v>1</v>
       </c>
-      <c r="C161" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C161" s="1"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
@@ -3165,9 +2837,7 @@
       <c r="B162" s="2">
         <v>1</v>
       </c>
-      <c r="C162" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C162" s="1"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
@@ -3176,9 +2846,7 @@
       <c r="B163" s="2">
         <v>1</v>
       </c>
-      <c r="C163" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C163" s="1"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
@@ -3187,9 +2855,7 @@
       <c r="B164" s="2">
         <v>1</v>
       </c>
-      <c r="C164" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C164" s="1"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
@@ -3198,9 +2864,7 @@
       <c r="B165" s="2">
         <v>1</v>
       </c>
-      <c r="C165" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C165" s="1"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
@@ -3209,9 +2873,7 @@
       <c r="B166" s="2">
         <v>1</v>
       </c>
-      <c r="C166" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C166" s="1"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
@@ -3220,9 +2882,7 @@
       <c r="B167" s="2">
         <v>1</v>
       </c>
-      <c r="C167" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C167" s="1"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
@@ -3231,9 +2891,7 @@
       <c r="B168" s="2">
         <v>1</v>
       </c>
-      <c r="C168" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C168" s="1"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
@@ -3242,9 +2900,7 @@
       <c r="B169" s="2">
         <v>1</v>
       </c>
-      <c r="C169" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C169" s="1"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
@@ -3253,9 +2909,7 @@
       <c r="B170" s="2">
         <v>1</v>
       </c>
-      <c r="C170" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C170" s="1"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
@@ -3264,9 +2918,7 @@
       <c r="B171" s="2">
         <v>1</v>
       </c>
-      <c r="C171" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C171" s="1"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
@@ -3275,9 +2927,7 @@
       <c r="B172" s="2">
         <v>1</v>
       </c>
-      <c r="C172" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C172" s="1"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
@@ -3286,9 +2936,7 @@
       <c r="B173" s="2">
         <v>1</v>
       </c>
-      <c r="C173" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C173" s="1"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
@@ -3297,9 +2945,7 @@
       <c r="B174" s="2">
         <v>1</v>
       </c>
-      <c r="C174" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C174" s="1"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
@@ -3308,9 +2954,7 @@
       <c r="B175" s="2">
         <v>1</v>
       </c>
-      <c r="C175" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C175" s="1"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
@@ -3319,9 +2963,7 @@
       <c r="B176" s="2">
         <v>1</v>
       </c>
-      <c r="C176" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C176" s="1"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
@@ -3330,9 +2972,7 @@
       <c r="B177" s="2">
         <v>1</v>
       </c>
-      <c r="C177" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C177" s="1"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
@@ -3341,9 +2981,7 @@
       <c r="B178" s="2">
         <v>1</v>
       </c>
-      <c r="C178" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C178" s="1"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
@@ -3352,9 +2990,7 @@
       <c r="B179" s="2">
         <v>1</v>
       </c>
-      <c r="C179" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C179" s="1"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
@@ -3363,9 +2999,7 @@
       <c r="B180" s="2">
         <v>1</v>
       </c>
-      <c r="C180" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C180" s="1"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
@@ -3374,9 +3008,7 @@
       <c r="B181" s="2">
         <v>1</v>
       </c>
-      <c r="C181" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C181" s="1"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
@@ -3385,9 +3017,7 @@
       <c r="B182" s="2">
         <v>1</v>
       </c>
-      <c r="C182" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C182" s="1"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
@@ -3396,9 +3026,7 @@
       <c r="B183" s="2">
         <v>1</v>
       </c>
-      <c r="C183" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C183" s="1"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
@@ -3407,9 +3035,7 @@
       <c r="B184" s="2">
         <v>1</v>
       </c>
-      <c r="C184" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C184" s="1"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
@@ -3418,9 +3044,7 @@
       <c r="B185" s="2">
         <v>1</v>
       </c>
-      <c r="C185" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C185" s="1"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
@@ -3429,9 +3053,7 @@
       <c r="B186" s="2">
         <v>1</v>
       </c>
-      <c r="C186" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C186" s="1"/>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
@@ -3440,9 +3062,7 @@
       <c r="B187" s="2">
         <v>1</v>
       </c>
-      <c r="C187" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C187" s="1"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
@@ -3451,9 +3071,7 @@
       <c r="B188" s="2">
         <v>1</v>
       </c>
-      <c r="C188" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C188" s="1"/>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
@@ -3462,9 +3080,7 @@
       <c r="B189" s="2">
         <v>1</v>
       </c>
-      <c r="C189" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C189" s="1"/>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
@@ -3473,9 +3089,7 @@
       <c r="B190" s="2">
         <v>1</v>
       </c>
-      <c r="C190" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C190" s="1"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
@@ -3484,9 +3098,7 @@
       <c r="B191" s="2">
         <v>1</v>
       </c>
-      <c r="C191" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C191" s="1"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
@@ -3495,9 +3107,7 @@
       <c r="B192" s="2">
         <v>1</v>
       </c>
-      <c r="C192" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C192" s="1"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
@@ -3506,9 +3116,7 @@
       <c r="B193" s="2">
         <v>1</v>
       </c>
-      <c r="C193" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C193" s="1"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
@@ -3517,9 +3125,7 @@
       <c r="B194" s="2">
         <v>1</v>
       </c>
-      <c r="C194" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C194" s="1"/>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
@@ -3528,9 +3134,7 @@
       <c r="B195" s="2">
         <v>1</v>
       </c>
-      <c r="C195" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C195" s="1"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
@@ -3539,9 +3143,7 @@
       <c r="B196" s="2">
         <v>1</v>
       </c>
-      <c r="C196" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C196" s="1"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
@@ -3550,9 +3152,7 @@
       <c r="B197" s="2">
         <v>1</v>
       </c>
-      <c r="C197" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C197" s="1"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
@@ -3561,9 +3161,7 @@
       <c r="B198" s="2">
         <v>1</v>
       </c>
-      <c r="C198" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C198" s="1"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
@@ -3572,9 +3170,7 @@
       <c r="B199" s="2">
         <v>1</v>
       </c>
-      <c r="C199" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C199" s="1"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
@@ -3583,9 +3179,7 @@
       <c r="B200" s="2">
         <v>1</v>
       </c>
-      <c r="C200" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C200" s="1"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
@@ -3594,9 +3188,7 @@
       <c r="B201" s="2">
         <v>1</v>
       </c>
-      <c r="C201" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C201" s="1"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
@@ -3605,9 +3197,7 @@
       <c r="B202" s="2">
         <v>1</v>
       </c>
-      <c r="C202" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C202" s="1"/>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
@@ -3616,9 +3206,7 @@
       <c r="B203" s="2">
         <v>1</v>
       </c>
-      <c r="C203" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C203" s="1"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
@@ -3627,9 +3215,7 @@
       <c r="B204" s="2">
         <v>1</v>
       </c>
-      <c r="C204" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C204" s="1"/>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
@@ -3638,9 +3224,7 @@
       <c r="B205" s="2">
         <v>1</v>
       </c>
-      <c r="C205" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C205" s="1"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
@@ -3649,9 +3233,7 @@
       <c r="B206" s="2">
         <v>1</v>
       </c>
-      <c r="C206" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C206" s="1"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
@@ -3660,9 +3242,7 @@
       <c r="B207" s="2">
         <v>1</v>
       </c>
-      <c r="C207" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C207" s="1"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
@@ -3671,9 +3251,7 @@
       <c r="B208" s="2">
         <v>1</v>
       </c>
-      <c r="C208" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C208" s="1"/>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
@@ -3682,9 +3260,7 @@
       <c r="B209" s="2">
         <v>1</v>
       </c>
-      <c r="C209" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C209" s="1"/>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
@@ -3693,9 +3269,7 @@
       <c r="B210" s="2">
         <v>1</v>
       </c>
-      <c r="C210" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C210" s="1"/>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
@@ -3704,9 +3278,7 @@
       <c r="B211" s="2">
         <v>1</v>
       </c>
-      <c r="C211" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C211" s="1"/>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
@@ -3715,9 +3287,7 @@
       <c r="B212" s="2">
         <v>1</v>
       </c>
-      <c r="C212" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C212" s="1"/>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
@@ -3726,9 +3296,7 @@
       <c r="B213" s="2">
         <v>1</v>
       </c>
-      <c r="C213" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C213" s="1"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
@@ -3737,9 +3305,7 @@
       <c r="B214" s="2">
         <v>1</v>
       </c>
-      <c r="C214" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C214" s="1"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
@@ -3748,9 +3314,7 @@
       <c r="B215" s="2">
         <v>1</v>
       </c>
-      <c r="C215" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C215" s="1"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
@@ -3759,9 +3323,7 @@
       <c r="B216" s="2">
         <v>1</v>
       </c>
-      <c r="C216" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C216" s="1"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
@@ -3770,9 +3332,7 @@
       <c r="B217" s="2">
         <v>1</v>
       </c>
-      <c r="C217" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C217" s="1"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
@@ -3781,9 +3341,7 @@
       <c r="B218" s="2">
         <v>1</v>
       </c>
-      <c r="C218" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C218" s="1"/>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
@@ -3792,9 +3350,7 @@
       <c r="B219" s="2">
         <v>1</v>
       </c>
-      <c r="C219" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C219" s="1"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
@@ -3803,9 +3359,7 @@
       <c r="B220" s="2">
         <v>1</v>
       </c>
-      <c r="C220" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C220" s="1"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
@@ -3814,9 +3368,7 @@
       <c r="B221" s="2">
         <v>1</v>
       </c>
-      <c r="C221" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C221" s="1"/>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
@@ -3825,9 +3377,7 @@
       <c r="B222" s="2">
         <v>1</v>
       </c>
-      <c r="C222" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C222" s="1"/>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
@@ -3836,9 +3386,7 @@
       <c r="B223" s="2">
         <v>1</v>
       </c>
-      <c r="C223" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C223" s="1"/>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
@@ -3847,9 +3395,7 @@
       <c r="B224" s="2">
         <v>1</v>
       </c>
-      <c r="C224" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C224" s="1"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
@@ -3858,9 +3404,7 @@
       <c r="B225" s="2">
         <v>1</v>
       </c>
-      <c r="C225" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C225" s="1"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
@@ -3869,9 +3413,7 @@
       <c r="B226" s="2">
         <v>1</v>
       </c>
-      <c r="C226" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C226" s="1"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
@@ -3880,9 +3422,7 @@
       <c r="B227" s="2">
         <v>1</v>
       </c>
-      <c r="C227" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C227" s="1"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
@@ -3891,9 +3431,7 @@
       <c r="B228" s="2">
         <v>1</v>
       </c>
-      <c r="C228" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C228" s="1"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
@@ -3902,9 +3440,7 @@
       <c r="B229" s="2">
         <v>1</v>
       </c>
-      <c r="C229" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C229" s="1"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
@@ -3913,9 +3449,7 @@
       <c r="B230" s="2">
         <v>1</v>
       </c>
-      <c r="C230" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C230" s="1"/>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
@@ -3924,9 +3458,7 @@
       <c r="B231" s="2">
         <v>1</v>
       </c>
-      <c r="C231" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C231" s="1"/>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
@@ -3935,9 +3467,7 @@
       <c r="B232" s="2">
         <v>1</v>
       </c>
-      <c r="C232" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C232" s="1"/>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
@@ -3946,9 +3476,7 @@
       <c r="B233" s="2">
         <v>1</v>
       </c>
-      <c r="C233" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C233" s="1"/>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
@@ -3957,9 +3485,7 @@
       <c r="B234" s="2">
         <v>1</v>
       </c>
-      <c r="C234" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C234" s="1"/>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
@@ -3968,9 +3494,7 @@
       <c r="B235" s="2">
         <v>1</v>
       </c>
-      <c r="C235" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C235" s="1"/>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
@@ -3979,9 +3503,7 @@
       <c r="B236" s="2">
         <v>1</v>
       </c>
-      <c r="C236" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C236" s="1"/>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
@@ -3990,9 +3512,7 @@
       <c r="B237" s="2">
         <v>1</v>
       </c>
-      <c r="C237" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C237" s="1"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
@@ -4001,9 +3521,7 @@
       <c r="B238" s="2">
         <v>1</v>
       </c>
-      <c r="C238" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C238" s="1"/>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
@@ -4012,9 +3530,7 @@
       <c r="B239" s="2">
         <v>1</v>
       </c>
-      <c r="C239" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C239" s="1"/>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
@@ -4023,9 +3539,7 @@
       <c r="B240" s="2">
         <v>1</v>
       </c>
-      <c r="C240" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C240" s="1"/>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
@@ -4034,9 +3548,7 @@
       <c r="B241" s="2">
         <v>1</v>
       </c>
-      <c r="C241" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C241" s="1"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
@@ -4045,9 +3557,7 @@
       <c r="B242" s="2">
         <v>1</v>
       </c>
-      <c r="C242" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C242" s="1"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
@@ -4056,9 +3566,7 @@
       <c r="B243" s="2">
         <v>1</v>
       </c>
-      <c r="C243" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C243" s="1"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
@@ -4067,9 +3575,7 @@
       <c r="B244" s="2">
         <v>1</v>
       </c>
-      <c r="C244" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C244" s="1"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
@@ -4078,9 +3584,7 @@
       <c r="B245" s="2">
         <v>1</v>
       </c>
-      <c r="C245" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C245" s="1"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
@@ -4089,9 +3593,7 @@
       <c r="B246" s="2">
         <v>1</v>
       </c>
-      <c r="C246" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C246" s="1"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
@@ -4100,9 +3602,7 @@
       <c r="B247" s="2">
         <v>1</v>
       </c>
-      <c r="C247" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C247" s="1"/>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
@@ -4111,9 +3611,7 @@
       <c r="B248" s="2">
         <v>1</v>
       </c>
-      <c r="C248" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C248" s="1"/>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
@@ -4122,9 +3620,7 @@
       <c r="B249" s="2">
         <v>1</v>
       </c>
-      <c r="C249" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C249" s="1"/>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
@@ -4133,9 +3629,7 @@
       <c r="B250" s="2">
         <v>1</v>
       </c>
-      <c r="C250" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C250" s="1"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
@@ -4144,9 +3638,7 @@
       <c r="B251" s="2">
         <v>1</v>
       </c>
-      <c r="C251" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C251" s="1"/>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
@@ -4155,9 +3647,7 @@
       <c r="B252" s="2">
         <v>1</v>
       </c>
-      <c r="C252" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C252" s="1"/>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
@@ -4166,9 +3656,7 @@
       <c r="B253" s="2">
         <v>1</v>
       </c>
-      <c r="C253" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C253" s="1"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
@@ -4177,9 +3665,7 @@
       <c r="B254" s="2">
         <v>1</v>
       </c>
-      <c r="C254" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C254" s="1"/>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
@@ -4188,9 +3674,7 @@
       <c r="B255" s="2">
         <v>1</v>
       </c>
-      <c r="C255" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C255" s="1"/>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
@@ -4199,9 +3683,7 @@
       <c r="B256" s="2">
         <v>1</v>
       </c>
-      <c r="C256" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C256" s="1"/>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="1" t="s">
@@ -4210,9 +3692,7 @@
       <c r="B257" s="2">
         <v>1</v>
       </c>
-      <c r="C257" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C257" s="1"/>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
@@ -4221,9 +3701,7 @@
       <c r="B258" s="2">
         <v>1</v>
       </c>
-      <c r="C258" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C258" s="1"/>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="1" t="s">
@@ -4232,9 +3710,7 @@
       <c r="B259" s="2">
         <v>1</v>
       </c>
-      <c r="C259" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C259" s="1"/>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
@@ -4243,9 +3719,7 @@
       <c r="B260" s="2">
         <v>1</v>
       </c>
-      <c r="C260" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C260" s="1"/>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
@@ -4254,9 +3728,7 @@
       <c r="B261" s="2">
         <v>1</v>
       </c>
-      <c r="C261" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C261" s="1"/>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
@@ -4265,9 +3737,7 @@
       <c r="B262" s="2">
         <v>1</v>
       </c>
-      <c r="C262" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C262" s="1"/>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
@@ -4276,9 +3746,7 @@
       <c r="B263" s="2">
         <v>1</v>
       </c>
-      <c r="C263" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C263" s="1"/>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
@@ -4287,9 +3755,7 @@
       <c r="B264" s="2">
         <v>1</v>
       </c>
-      <c r="C264" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C264" s="1"/>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
@@ -4298,9 +3764,7 @@
       <c r="B265" s="2">
         <v>1</v>
       </c>
-      <c r="C265" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C265" s="1"/>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
@@ -4309,9 +3773,7 @@
       <c r="B266" s="2">
         <v>1</v>
       </c>
-      <c r="C266" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C266" s="1"/>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
@@ -4320,9 +3782,7 @@
       <c r="B267" s="2">
         <v>1</v>
       </c>
-      <c r="C267" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C267" s="1"/>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
@@ -4331,9 +3791,7 @@
       <c r="B268" s="2">
         <v>1</v>
       </c>
-      <c r="C268" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C268" s="1"/>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
@@ -4342,9 +3800,7 @@
       <c r="B269" s="2">
         <v>1</v>
       </c>
-      <c r="C269" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C269" s="1"/>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
@@ -4353,9 +3809,7 @@
       <c r="B270" s="2">
         <v>1</v>
       </c>
-      <c r="C270" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C270" s="1"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
@@ -4364,9 +3818,7 @@
       <c r="B271" s="2">
         <v>1</v>
       </c>
-      <c r="C271" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C271" s="1"/>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
@@ -4375,9 +3827,7 @@
       <c r="B272" s="2">
         <v>1</v>
       </c>
-      <c r="C272" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C272" s="1"/>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
@@ -4386,9 +3836,7 @@
       <c r="B273" s="2">
         <v>1</v>
       </c>
-      <c r="C273" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C273" s="1"/>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
@@ -4397,9 +3845,7 @@
       <c r="B274" s="2">
         <v>1</v>
       </c>
-      <c r="C274" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C274" s="1"/>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
@@ -4408,9 +3854,7 @@
       <c r="B275" s="2">
         <v>1</v>
       </c>
-      <c r="C275" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C275" s="1"/>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
@@ -4419,9 +3863,7 @@
       <c r="B276" s="2">
         <v>1</v>
       </c>
-      <c r="C276" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C276" s="1"/>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
@@ -4430,9 +3872,7 @@
       <c r="B277" s="2">
         <v>1</v>
       </c>
-      <c r="C277" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C277" s="1"/>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
@@ -4441,9 +3881,7 @@
       <c r="B278" s="2">
         <v>1</v>
       </c>
-      <c r="C278" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C278" s="1"/>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
@@ -4452,9 +3890,7 @@
       <c r="B279" s="2">
         <v>1</v>
       </c>
-      <c r="C279" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C279" s="1"/>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
@@ -4463,9 +3899,7 @@
       <c r="B280" s="2">
         <v>1</v>
       </c>
-      <c r="C280" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C280" s="1"/>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
@@ -4474,9 +3908,7 @@
       <c r="B281" s="2">
         <v>1</v>
       </c>
-      <c r="C281" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C281" s="1"/>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
@@ -4485,9 +3917,7 @@
       <c r="B282" s="2">
         <v>1</v>
       </c>
-      <c r="C282" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C282" s="1"/>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
@@ -4496,9 +3926,7 @@
       <c r="B283" s="2">
         <v>1</v>
       </c>
-      <c r="C283" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C283" s="1"/>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
@@ -4507,9 +3935,7 @@
       <c r="B284" s="2">
         <v>1</v>
       </c>
-      <c r="C284" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C284" s="1"/>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
@@ -4518,9 +3944,7 @@
       <c r="B285" s="2">
         <v>1</v>
       </c>
-      <c r="C285" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C285" s="1"/>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
@@ -4529,9 +3953,7 @@
       <c r="B286" s="2">
         <v>1</v>
       </c>
-      <c r="C286" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C286" s="1"/>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
@@ -4540,9 +3962,7 @@
       <c r="B287" s="2">
         <v>1</v>
       </c>
-      <c r="C287" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C287" s="1"/>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
@@ -4551,9 +3971,7 @@
       <c r="B288" s="2">
         <v>1</v>
       </c>
-      <c r="C288" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C288" s="1"/>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
@@ -4562,9 +3980,7 @@
       <c r="B289" s="2">
         <v>1</v>
       </c>
-      <c r="C289" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C289" s="1"/>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
@@ -4573,9 +3989,7 @@
       <c r="B290" s="2">
         <v>1</v>
       </c>
-      <c r="C290" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C290" s="1"/>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
@@ -4584,9 +3998,7 @@
       <c r="B291" s="2">
         <v>1</v>
       </c>
-      <c r="C291" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C291" s="1"/>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" s="1" t="s">
@@ -4595,9 +4007,7 @@
       <c r="B292" s="2">
         <v>1</v>
       </c>
-      <c r="C292" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C292" s="1"/>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
@@ -4606,9 +4016,7 @@
       <c r="B293" s="2">
         <v>1</v>
       </c>
-      <c r="C293" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C293" s="1"/>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" s="1" t="s">
@@ -4617,9 +4025,7 @@
       <c r="B294" s="2">
         <v>1</v>
       </c>
-      <c r="C294" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C294" s="1"/>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" s="1" t="s">
@@ -4628,9 +4034,7 @@
       <c r="B295" s="2">
         <v>1</v>
       </c>
-      <c r="C295" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C295" s="1"/>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" s="1" t="s">
@@ -4639,9 +4043,7 @@
       <c r="B296" s="2">
         <v>1</v>
       </c>
-      <c r="C296" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C296" s="1"/>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" s="1" t="s">
@@ -4650,9 +4052,7 @@
       <c r="B297" s="2">
         <v>1</v>
       </c>
-      <c r="C297" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C297" s="1"/>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="1" t="s">
@@ -4661,9 +4061,7 @@
       <c r="B298" s="2">
         <v>1</v>
       </c>
-      <c r="C298" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C298" s="1"/>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="1" t="s">
@@ -4672,9 +4070,7 @@
       <c r="B299" s="2">
         <v>1</v>
       </c>
-      <c r="C299" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C299" s="1"/>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" s="1" t="s">
@@ -4683,9 +4079,7 @@
       <c r="B300" s="2">
         <v>1</v>
       </c>
-      <c r="C300" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C300" s="1"/>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="1" t="s">
@@ -4694,9 +4088,7 @@
       <c r="B301" s="2">
         <v>1</v>
       </c>
-      <c r="C301" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C301" s="1"/>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="1" t="s">
@@ -4705,9 +4097,7 @@
       <c r="B302" s="2">
         <v>1</v>
       </c>
-      <c r="C302" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C302" s="1"/>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="1" t="s">
@@ -4716,9 +4106,7 @@
       <c r="B303" s="2">
         <v>1</v>
       </c>
-      <c r="C303" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C303" s="1"/>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" s="1" t="s">
@@ -4727,9 +4115,7 @@
       <c r="B304" s="2">
         <v>1</v>
       </c>
-      <c r="C304" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C304" s="1"/>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" s="1" t="s">
@@ -4738,9 +4124,7 @@
       <c r="B305" s="2">
         <v>1</v>
       </c>
-      <c r="C305" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C305" s="1"/>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
@@ -4749,9 +4133,7 @@
       <c r="B306" s="2">
         <v>1</v>
       </c>
-      <c r="C306" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C306" s="1"/>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" s="1" t="s">
@@ -4760,9 +4142,7 @@
       <c r="B307" s="2">
         <v>1</v>
       </c>
-      <c r="C307" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C307" s="1"/>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" s="1" t="s">
@@ -4771,9 +4151,7 @@
       <c r="B308" s="2">
         <v>1</v>
       </c>
-      <c r="C308" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C308" s="1"/>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" s="1" t="s">
@@ -4782,9 +4160,7 @@
       <c r="B309" s="2">
         <v>1</v>
       </c>
-      <c r="C309" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C309" s="1"/>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" s="1" t="s">
@@ -4793,9 +4169,7 @@
       <c r="B310" s="2">
         <v>1</v>
       </c>
-      <c r="C310" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C310" s="1"/>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311" s="1" t="s">
@@ -4804,9 +4178,7 @@
       <c r="B311" s="2">
         <v>1</v>
       </c>
-      <c r="C311" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C311" s="1"/>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312" s="1" t="s">
@@ -4815,9 +4187,7 @@
       <c r="B312" s="2">
         <v>1</v>
       </c>
-      <c r="C312" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C312" s="1"/>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="1" t="s">
@@ -4826,9 +4196,7 @@
       <c r="B313" s="2">
         <v>1</v>
       </c>
-      <c r="C313" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C313" s="1"/>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314" s="1" t="s">
@@ -4837,9 +4205,7 @@
       <c r="B314" s="2">
         <v>1</v>
       </c>
-      <c r="C314" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C314" s="1"/>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="1" t="s">
@@ -4848,9 +4214,7 @@
       <c r="B315" s="2">
         <v>1</v>
       </c>
-      <c r="C315" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C315" s="1"/>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="1" t="s">
@@ -4859,9 +4223,7 @@
       <c r="B316" s="2">
         <v>1</v>
       </c>
-      <c r="C316" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C316" s="1"/>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="1" t="s">
@@ -4870,9 +4232,7 @@
       <c r="B317" s="2">
         <v>1</v>
       </c>
-      <c r="C317" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C317" s="1"/>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" s="1" t="s">
@@ -4881,9 +4241,7 @@
       <c r="B318" s="2">
         <v>1</v>
       </c>
-      <c r="C318" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C318" s="1"/>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="1" t="s">
@@ -4892,9 +4250,7 @@
       <c r="B319" s="2">
         <v>1</v>
       </c>
-      <c r="C319" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C319" s="1"/>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="1" t="s">
@@ -4903,9 +4259,7 @@
       <c r="B320" s="2">
         <v>1</v>
       </c>
-      <c r="C320" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C320" s="1"/>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321" s="1" t="s">
@@ -4914,9 +4268,7 @@
       <c r="B321" s="2">
         <v>1</v>
       </c>
-      <c r="C321" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C321" s="1"/>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="1" t="s">
@@ -4925,9 +4277,7 @@
       <c r="B322" s="2">
         <v>1</v>
       </c>
-      <c r="C322" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C322" s="1"/>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323" s="1" t="s">
@@ -4936,9 +4286,7 @@
       <c r="B323" s="2">
         <v>1</v>
       </c>
-      <c r="C323" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C323" s="1"/>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324" s="1" t="s">
@@ -4947,9 +4295,7 @@
       <c r="B324" s="2">
         <v>1</v>
       </c>
-      <c r="C324" s="1" t="s">
-        <v>324</v>
-      </c>
+      <c r="C324" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>